<commit_message>
Regretion Run SCD0021 - Abnormal Upload List File and Assign, SCD0023 - Active dan Inactive pada list file, SCD0024 - Download File, SCD0025 - Download File, SCD0026 - Membuka Gembok, and SCD0027 - Mengunci Gembok
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0026 - Membuka Gembok.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0026 - Membuka Gembok.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\Digisales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0AC19E-1692-4209-84FF-67F69B059199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D681D67-1D0D-4514-865B-121D022F603F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0026" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Link download file menjadi enabled</t>
+  </si>
+  <si>
+    <t>Wilayah_05_202206_31.zip</t>
   </si>
 </sst>
 </file>
@@ -524,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +549,7 @@
     <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.7109375" customWidth="1"/>
-    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -639,7 +642,9 @@
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
@@ -674,7 +679,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5">
-        <v>1121</v>
+        <v>1177</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>

</xml_diff>